<commit_message>
Updates to documentation and Cytoscape version corrections
Several updates to the documentation and style files to correct it for the Cytoscape 3.7 and use of CyAnimator.
</commit_message>
<xml_diff>
--- a/Netflux/models/exampleNet.xlsx
+++ b/Netflux/models/exampleNet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="360" windowWidth="11715" windowHeight="9525"/>
+    <workbookView xWindow="195" yWindow="360" windowWidth="11715" windowHeight="9525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="species" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -180,15 +180,12 @@
   </si>
   <si>
     <t>middle</t>
-  </si>
-  <si>
-    <t>D &amp; !A =&gt; D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -321,6 +318,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -368,7 +368,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -403,7 +403,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -614,24 +614,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="56.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.1328125" customWidth="1"/>
+    <col min="2" max="2" width="10.86328125" customWidth="1"/>
+    <col min="3" max="3" width="56.73046875" customWidth="1"/>
+    <col min="7" max="7" width="15.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -663,7 +663,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>30</v>
       </c>
@@ -684,7 +684,7 @@
       </c>
       <c r="I3" s="17"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>31</v>
       </c>
@@ -705,7 +705,7 @@
       </c>
       <c r="I4" s="17"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>32</v>
       </c>
@@ -726,7 +726,7 @@
       </c>
       <c r="I5" s="17"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>33</v>
       </c>
@@ -747,7 +747,7 @@
       </c>
       <c r="I6" s="17"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>34</v>
       </c>
@@ -768,415 +768,415 @@
       </c>
       <c r="I7" s="17"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="G8" s="15"/>
       <c r="I8" s="17"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="G9" s="15"/>
       <c r="I9" s="17"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="G10" s="16"/>
       <c r="I10" s="17"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="G11" s="16"/>
       <c r="I11" s="17"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="G12" s="16"/>
       <c r="I12" s="17"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="G13" s="16"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="G14" s="16"/>
       <c r="I14" s="17"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="G15" s="16"/>
       <c r="I15" s="17"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C16" s="6"/>
       <c r="G16" s="16"/>
       <c r="I16" s="17"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G17" s="16"/>
       <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G18" s="16"/>
       <c r="I18" s="17"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G19" s="16"/>
       <c r="I19" s="17"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G20" s="16"/>
       <c r="I20" s="17"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G21" s="16"/>
       <c r="I21" s="17"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G22" s="16"/>
       <c r="I22" s="17"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G23" s="16"/>
       <c r="I23" s="17"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G24" s="15"/>
       <c r="I24" s="17"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G25" s="15"/>
       <c r="I25" s="17"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G26" s="15"/>
       <c r="I26" s="17"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G27" s="15"/>
       <c r="I27" s="17"/>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G28" s="15"/>
       <c r="I28" s="17"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G29" s="15"/>
       <c r="I29" s="17"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B30" s="6"/>
       <c r="G30" s="15"/>
       <c r="I30" s="6"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G31" s="15"/>
       <c r="I31" s="17"/>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G32" s="15"/>
       <c r="I32" s="17"/>
     </row>
-    <row r="33" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G33" s="15"/>
       <c r="I33" s="17"/>
     </row>
-    <row r="34" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G34" s="15"/>
       <c r="I34" s="17"/>
     </row>
-    <row r="35" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G35" s="15"/>
       <c r="I35" s="17"/>
     </row>
-    <row r="36" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G36" s="15"/>
       <c r="I36" s="17"/>
     </row>
-    <row r="37" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G37" s="15"/>
       <c r="I37" s="17"/>
     </row>
-    <row r="38" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G38" s="15"/>
       <c r="I38" s="17"/>
     </row>
-    <row r="39" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G39" s="15"/>
       <c r="I39" s="17"/>
     </row>
-    <row r="40" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G40" s="15"/>
       <c r="I40" s="17"/>
     </row>
-    <row r="41" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G41" s="15"/>
       <c r="I41" s="17"/>
     </row>
-    <row r="42" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G42" s="15"/>
       <c r="I42" s="17"/>
     </row>
-    <row r="43" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G43" s="15"/>
       <c r="I43" s="17"/>
     </row>
-    <row r="44" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G44" s="15"/>
       <c r="I44" s="17"/>
     </row>
-    <row r="45" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G45" s="15"/>
       <c r="I45" s="17"/>
     </row>
-    <row r="46" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G46" s="15"/>
       <c r="I46" s="17"/>
     </row>
-    <row r="47" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G47" s="15"/>
       <c r="I47" s="17"/>
     </row>
-    <row r="48" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G48" s="15"/>
       <c r="I48" s="17"/>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G49" s="15"/>
       <c r="I49" s="17"/>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G50" s="15"/>
       <c r="I50" s="17"/>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G51" s="15"/>
       <c r="I51" s="17"/>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G52" s="15"/>
       <c r="I52" s="17"/>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G53" s="15"/>
       <c r="I53" s="17"/>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G54" s="15"/>
       <c r="I54" s="17"/>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G55" s="15"/>
       <c r="I55" s="17"/>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G56" s="15"/>
       <c r="I56" s="17"/>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G57" s="15"/>
       <c r="I57" s="17"/>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
       <c r="G58" s="16"/>
       <c r="I58" s="6"/>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G59" s="15"/>
       <c r="I59" s="17"/>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G60" s="15"/>
       <c r="I60" s="17"/>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G61" s="15"/>
       <c r="I61" s="17"/>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G62" s="15"/>
       <c r="I62" s="17"/>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G63" s="15"/>
       <c r="I63" s="17"/>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G64" s="15"/>
       <c r="I64" s="17"/>
     </row>
-    <row r="65" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G65" s="15"/>
       <c r="I65" s="17"/>
     </row>
-    <row r="66" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G66" s="15"/>
       <c r="I66" s="17"/>
     </row>
-    <row r="67" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G67" s="15"/>
       <c r="I67" s="17"/>
     </row>
-    <row r="68" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G68" s="15"/>
       <c r="I68" s="17"/>
     </row>
-    <row r="69" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G69" s="15"/>
       <c r="I69" s="17"/>
     </row>
-    <row r="70" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G70" s="15"/>
       <c r="I70" s="17"/>
     </row>
-    <row r="71" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G71" s="15"/>
       <c r="I71" s="17"/>
     </row>
-    <row r="72" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G72" s="15"/>
       <c r="I72" s="17"/>
     </row>
-    <row r="73" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G73" s="15"/>
       <c r="I73" s="17"/>
     </row>
-    <row r="74" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G74" s="15"/>
       <c r="I74" s="17"/>
     </row>
-    <row r="75" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G75" s="15"/>
       <c r="I75" s="17"/>
     </row>
-    <row r="76" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G76" s="15"/>
       <c r="I76" s="17"/>
     </row>
-    <row r="77" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G77" s="15"/>
       <c r="I77" s="17"/>
     </row>
-    <row r="78" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G78" s="15"/>
       <c r="I78" s="17"/>
     </row>
-    <row r="79" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G79" s="15"/>
       <c r="I79" s="17"/>
     </row>
-    <row r="80" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G80" s="15"/>
       <c r="I80" s="17"/>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G81" s="15"/>
       <c r="I81" s="17"/>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G82" s="15"/>
       <c r="I82" s="17"/>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G83" s="15"/>
       <c r="I83" s="17"/>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G84" s="15"/>
       <c r="I84" s="17"/>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G85" s="15"/>
       <c r="I85" s="17"/>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G86" s="15"/>
       <c r="I86" s="17"/>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G87" s="15"/>
       <c r="I87" s="17"/>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G88" s="15"/>
       <c r="I88" s="17"/>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G89" s="15"/>
       <c r="I89" s="17"/>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G90" s="15"/>
       <c r="I90" s="17"/>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G91" s="15"/>
       <c r="I91" s="17"/>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G92" s="15"/>
       <c r="I92" s="17"/>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G93" s="15"/>
       <c r="I93" s="17"/>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G94" s="15"/>
       <c r="I94" s="17"/>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.45">
       <c r="G95" s="15"/>
       <c r="I95" s="17"/>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
       <c r="G96" s="15"/>
       <c r="I96" s="6"/>
     </row>
-    <row r="97" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G97" s="15"/>
       <c r="I97" s="17"/>
     </row>
-    <row r="98" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G98" s="15"/>
       <c r="I98" s="17"/>
     </row>
-    <row r="99" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G99" s="15"/>
       <c r="I99" s="17"/>
     </row>
-    <row r="100" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G100" s="15"/>
       <c r="I100" s="17"/>
     </row>
-    <row r="101" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G101" s="15"/>
       <c r="I101" s="17"/>
     </row>
-    <row r="102" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G102" s="15"/>
       <c r="I102" s="17"/>
     </row>
-    <row r="103" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G103" s="15"/>
       <c r="I103" s="17"/>
     </row>
-    <row r="104" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G104" s="15"/>
       <c r="I104" s="17"/>
     </row>
-    <row r="105" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G105" s="15"/>
       <c r="I105" s="17"/>
     </row>
-    <row r="106" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G106" s="15"/>
       <c r="I106" s="17"/>
     </row>
-    <row r="107" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G107" s="15"/>
       <c r="I107" s="17"/>
     </row>
-    <row r="108" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="7:9" x14ac:dyDescent="0.45">
       <c r="G108" s="15"/>
       <c r="I108" s="17"/>
     </row>
@@ -1196,29 +1196,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T193"/>
+  <dimension ref="A1:T192"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="44.7109375" customWidth="1"/>
-    <col min="4" max="6" width="8.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="10" width="9.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" customWidth="1"/>
+    <col min="3" max="3" width="44.73046875" customWidth="1"/>
+    <col min="4" max="6" width="8.265625" customWidth="1"/>
+    <col min="7" max="7" width="12.73046875" customWidth="1"/>
+    <col min="8" max="8" width="13.265625" customWidth="1"/>
+    <col min="9" max="10" width="9.73046875" customWidth="1"/>
+    <col min="11" max="11" width="11.59765625" customWidth="1"/>
+    <col min="14" max="14" width="13.3984375" customWidth="1"/>
+    <col min="15" max="15" width="10.86328125" customWidth="1"/>
+    <col min="16" max="16" width="10.1328125" customWidth="1"/>
+    <col min="17" max="17" width="11.73046875" customWidth="1"/>
+    <col min="18" max="18" width="9.59765625" customWidth="1"/>
     <col min="20" max="20" width="171" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -1226,7 +1226,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -1408,73 +1408,63 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1.4</v>
-      </c>
-      <c r="F9">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.45">
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.45">
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.45">
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.45">
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.45">
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.45">
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="L18" s="7"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
+    <row r="17" spans="3:20" x14ac:dyDescent="0.45">
+      <c r="L17" s="7"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="6"/>
+    </row>
+    <row r="18" spans="3:20" x14ac:dyDescent="0.45">
+      <c r="C18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
       <c r="Q18" s="6"/>
       <c r="S18" s="8"/>
       <c r="T18" s="6"/>
     </row>
-    <row r="19" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="9"/>
       <c r="M19" s="8"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
       <c r="S19" s="8"/>
       <c r="T19" s="6"/>
     </row>
-    <row r="20" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C20" s="6"/>
       <c r="M20" s="8"/>
       <c r="N20" s="6"/>
@@ -1484,52 +1474,54 @@
       <c r="S20" s="8"/>
       <c r="T20" s="6"/>
     </row>
-    <row r="21" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C21" s="6"/>
-      <c r="M21" s="8"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
-      <c r="S21" s="8"/>
+      <c r="R21" s="6"/>
       <c r="T21" s="6"/>
     </row>
-    <row r="22" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="8"/>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
+      <c r="S22" s="8"/>
       <c r="T22" s="6"/>
     </row>
-    <row r="23" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="8"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
       <c r="Q23" s="6"/>
       <c r="S23" s="8"/>
       <c r="T23" s="6"/>
     </row>
-    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
+    <row r="24" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L24" s="6"/>
       <c r="M24" s="8"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
       <c r="S24" s="8"/>
       <c r="T24" s="6"/>
     </row>
-    <row r="25" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:20" x14ac:dyDescent="0.45">
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
       <c r="L25" s="6"/>
       <c r="M25" s="8"/>
       <c r="N25" s="6"/>
@@ -1539,21 +1531,22 @@
       <c r="S25" s="8"/>
       <c r="T25" s="6"/>
     </row>
-    <row r="26" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
+    <row r="26" spans="3:20" x14ac:dyDescent="0.45">
+      <c r="C26" s="6"/>
+      <c r="L26" s="11"/>
       <c r="M26" s="8"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
       <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
       <c r="S26" s="8"/>
       <c r="T26" s="6"/>
     </row>
-    <row r="27" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C27" s="6"/>
-      <c r="L27" s="11"/>
+    <row r="27" spans="3:20" x14ac:dyDescent="0.45">
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="9"/>
       <c r="M27" s="8"/>
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
@@ -1563,31 +1556,27 @@
       <c r="S27" s="8"/>
       <c r="T27" s="6"/>
     </row>
-    <row r="28" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
+    <row r="28" spans="3:20" x14ac:dyDescent="0.45">
+      <c r="H28" s="7"/>
       <c r="L28" s="9"/>
       <c r="M28" s="8"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
       <c r="P28" s="10"/>
       <c r="Q28" s="6"/>
-      <c r="R28" s="6"/>
       <c r="S28" s="8"/>
       <c r="T28" s="6"/>
     </row>
-    <row r="29" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="H29" s="7"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
+    <row r="29" spans="3:20" x14ac:dyDescent="0.45">
+      <c r="L29" s="7"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
       <c r="Q29" s="6"/>
       <c r="S29" s="8"/>
       <c r="T29" s="6"/>
     </row>
-    <row r="30" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L30" s="7"/>
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
@@ -1596,8 +1585,11 @@
       <c r="S30" s="8"/>
       <c r="T30" s="6"/>
     </row>
-    <row r="31" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:20" x14ac:dyDescent="0.45">
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
       <c r="L31" s="7"/>
+      <c r="M31" s="8"/>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
@@ -1605,10 +1597,8 @@
       <c r="S31" s="8"/>
       <c r="T31" s="6"/>
     </row>
-    <row r="32" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="7"/>
+    <row r="32" spans="3:20" x14ac:dyDescent="0.45">
+      <c r="L32" s="6"/>
       <c r="M32" s="8"/>
       <c r="N32" s="6"/>
       <c r="O32" s="6"/>
@@ -1617,17 +1607,16 @@
       <c r="S32" s="8"/>
       <c r="T32" s="6"/>
     </row>
-    <row r="33" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="L33" s="6"/>
-      <c r="M33" s="8"/>
+    <row r="33" spans="9:20" x14ac:dyDescent="0.45">
+      <c r="L33" s="7"/>
       <c r="N33" s="6"/>
       <c r="O33" s="6"/>
       <c r="P33" s="6"/>
       <c r="Q33" s="6"/>
-      <c r="S33" s="8"/>
+      <c r="R33" s="6"/>
       <c r="T33" s="6"/>
     </row>
-    <row r="34" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="9:20" x14ac:dyDescent="0.45">
       <c r="L34" s="7"/>
       <c r="N34" s="6"/>
       <c r="O34" s="6"/>
@@ -1636,7 +1625,9 @@
       <c r="R34" s="6"/>
       <c r="T34" s="6"/>
     </row>
-    <row r="35" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="9:20" x14ac:dyDescent="0.45">
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
       <c r="L35" s="7"/>
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
@@ -1645,9 +1636,7 @@
       <c r="R35" s="6"/>
       <c r="T35" s="6"/>
     </row>
-    <row r="36" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
+    <row r="36" spans="9:20" x14ac:dyDescent="0.45">
       <c r="L36" s="7"/>
       <c r="N36" s="6"/>
       <c r="O36" s="6"/>
@@ -1656,7 +1645,7 @@
       <c r="R36" s="6"/>
       <c r="T36" s="6"/>
     </row>
-    <row r="37" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="9:20" x14ac:dyDescent="0.45">
       <c r="L37" s="7"/>
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
@@ -1665,7 +1654,7 @@
       <c r="R37" s="6"/>
       <c r="T37" s="6"/>
     </row>
-    <row r="38" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="9:20" x14ac:dyDescent="0.45">
       <c r="L38" s="7"/>
       <c r="N38" s="6"/>
       <c r="O38" s="6"/>
@@ -1674,7 +1663,7 @@
       <c r="R38" s="6"/>
       <c r="T38" s="6"/>
     </row>
-    <row r="39" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="9:20" x14ac:dyDescent="0.45">
       <c r="L39" s="7"/>
       <c r="N39" s="6"/>
       <c r="O39" s="6"/>
@@ -1683,7 +1672,7 @@
       <c r="R39" s="6"/>
       <c r="T39" s="6"/>
     </row>
-    <row r="40" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="9:20" x14ac:dyDescent="0.45">
       <c r="L40" s="7"/>
       <c r="N40" s="6"/>
       <c r="O40" s="6"/>
@@ -1692,8 +1681,7 @@
       <c r="R40" s="6"/>
       <c r="T40" s="6"/>
     </row>
-    <row r="41" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="L41" s="7"/>
+    <row r="41" spans="9:20" x14ac:dyDescent="0.45">
       <c r="N41" s="6"/>
       <c r="O41" s="6"/>
       <c r="P41" s="6"/>
@@ -1701,7 +1689,7 @@
       <c r="R41" s="6"/>
       <c r="T41" s="6"/>
     </row>
-    <row r="42" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="9:20" x14ac:dyDescent="0.45">
       <c r="N42" s="6"/>
       <c r="O42" s="6"/>
       <c r="P42" s="6"/>
@@ -1709,7 +1697,7 @@
       <c r="R42" s="6"/>
       <c r="T42" s="6"/>
     </row>
-    <row r="43" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="9:20" x14ac:dyDescent="0.45">
       <c r="N43" s="6"/>
       <c r="O43" s="6"/>
       <c r="P43" s="6"/>
@@ -1717,7 +1705,7 @@
       <c r="R43" s="6"/>
       <c r="T43" s="6"/>
     </row>
-    <row r="44" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="9:20" x14ac:dyDescent="0.45">
       <c r="N44" s="6"/>
       <c r="O44" s="6"/>
       <c r="P44" s="6"/>
@@ -1725,7 +1713,7 @@
       <c r="R44" s="6"/>
       <c r="T44" s="6"/>
     </row>
-    <row r="45" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="9:20" x14ac:dyDescent="0.45">
       <c r="N45" s="6"/>
       <c r="O45" s="6"/>
       <c r="P45" s="6"/>
@@ -1733,7 +1721,8 @@
       <c r="R45" s="6"/>
       <c r="T45" s="6"/>
     </row>
-    <row r="46" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="9:20" x14ac:dyDescent="0.45">
+      <c r="L46" s="7"/>
       <c r="N46" s="6"/>
       <c r="O46" s="6"/>
       <c r="P46" s="6"/>
@@ -1741,7 +1730,7 @@
       <c r="R46" s="6"/>
       <c r="T46" s="6"/>
     </row>
-    <row r="47" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="9:20" x14ac:dyDescent="0.45">
       <c r="L47" s="7"/>
       <c r="N47" s="6"/>
       <c r="O47" s="6"/>
@@ -1750,7 +1739,7 @@
       <c r="R47" s="6"/>
       <c r="T47" s="6"/>
     </row>
-    <row r="48" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="9:20" x14ac:dyDescent="0.45">
       <c r="L48" s="7"/>
       <c r="N48" s="6"/>
       <c r="O48" s="6"/>
@@ -1759,7 +1748,7 @@
       <c r="R48" s="6"/>
       <c r="T48" s="6"/>
     </row>
-    <row r="49" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L49" s="7"/>
       <c r="N49" s="6"/>
       <c r="O49" s="6"/>
@@ -1768,7 +1757,7 @@
       <c r="R49" s="6"/>
       <c r="T49" s="6"/>
     </row>
-    <row r="50" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L50" s="7"/>
       <c r="N50" s="6"/>
       <c r="O50" s="6"/>
@@ -1777,7 +1766,7 @@
       <c r="R50" s="6"/>
       <c r="T50" s="6"/>
     </row>
-    <row r="51" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L51" s="7"/>
       <c r="N51" s="6"/>
       <c r="O51" s="6"/>
@@ -1786,7 +1775,7 @@
       <c r="R51" s="6"/>
       <c r="T51" s="6"/>
     </row>
-    <row r="52" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L52" s="7"/>
       <c r="N52" s="6"/>
       <c r="O52" s="6"/>
@@ -1795,23 +1784,22 @@
       <c r="R52" s="6"/>
       <c r="T52" s="6"/>
     </row>
-    <row r="53" spans="12:20" x14ac:dyDescent="0.25">
-      <c r="L53" s="7"/>
+    <row r="53" spans="12:20" x14ac:dyDescent="0.45">
       <c r="N53" s="6"/>
       <c r="O53" s="6"/>
       <c r="P53" s="6"/>
       <c r="Q53" s="6"/>
-      <c r="R53" s="6"/>
       <c r="T53" s="6"/>
     </row>
-    <row r="54" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="12:20" x14ac:dyDescent="0.45">
       <c r="N54" s="6"/>
       <c r="O54" s="6"/>
       <c r="P54" s="6"/>
       <c r="Q54" s="6"/>
+      <c r="R54" s="6"/>
       <c r="T54" s="6"/>
     </row>
-    <row r="55" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="12:20" x14ac:dyDescent="0.45">
       <c r="N55" s="6"/>
       <c r="O55" s="6"/>
       <c r="P55" s="6"/>
@@ -1819,7 +1807,7 @@
       <c r="R55" s="6"/>
       <c r="T55" s="6"/>
     </row>
-    <row r="56" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="12:20" x14ac:dyDescent="0.45">
       <c r="N56" s="6"/>
       <c r="O56" s="6"/>
       <c r="P56" s="6"/>
@@ -1827,7 +1815,9 @@
       <c r="R56" s="6"/>
       <c r="T56" s="6"/>
     </row>
-    <row r="57" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="12:20" x14ac:dyDescent="0.45">
+      <c r="L57" s="7"/>
+      <c r="M57" s="8"/>
       <c r="N57" s="6"/>
       <c r="O57" s="6"/>
       <c r="P57" s="6"/>
@@ -1835,26 +1825,24 @@
       <c r="R57" s="6"/>
       <c r="T57" s="6"/>
     </row>
-    <row r="58" spans="12:20" x14ac:dyDescent="0.25">
-      <c r="L58" s="7"/>
-      <c r="M58" s="8"/>
+    <row r="58" spans="12:20" x14ac:dyDescent="0.45">
       <c r="N58" s="6"/>
       <c r="O58" s="6"/>
       <c r="P58" s="6"/>
       <c r="Q58" s="6"/>
-      <c r="R58" s="6"/>
       <c r="T58" s="6"/>
     </row>
-    <row r="59" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="12:20" x14ac:dyDescent="0.45">
+      <c r="L59" s="7"/>
+      <c r="M59" s="8"/>
       <c r="N59" s="6"/>
       <c r="O59" s="6"/>
       <c r="P59" s="6"/>
       <c r="Q59" s="6"/>
+      <c r="R59" s="6"/>
       <c r="T59" s="6"/>
     </row>
-    <row r="60" spans="12:20" x14ac:dyDescent="0.25">
-      <c r="L60" s="7"/>
-      <c r="M60" s="8"/>
+    <row r="60" spans="12:20" x14ac:dyDescent="0.45">
       <c r="N60" s="6"/>
       <c r="O60" s="6"/>
       <c r="P60" s="6"/>
@@ -1862,7 +1850,9 @@
       <c r="R60" s="6"/>
       <c r="T60" s="6"/>
     </row>
-    <row r="61" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="12:20" x14ac:dyDescent="0.45">
+      <c r="L61" s="7"/>
+      <c r="M61" s="8"/>
       <c r="N61" s="6"/>
       <c r="O61" s="6"/>
       <c r="P61" s="6"/>
@@ -1870,7 +1860,7 @@
       <c r="R61" s="6"/>
       <c r="T61" s="6"/>
     </row>
-    <row r="62" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L62" s="7"/>
       <c r="M62" s="8"/>
       <c r="N62" s="6"/>
@@ -1880,7 +1870,7 @@
       <c r="R62" s="6"/>
       <c r="T62" s="6"/>
     </row>
-    <row r="63" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L63" s="7"/>
       <c r="M63" s="8"/>
       <c r="N63" s="6"/>
@@ -1890,7 +1880,7 @@
       <c r="R63" s="6"/>
       <c r="T63" s="6"/>
     </row>
-    <row r="64" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L64" s="7"/>
       <c r="M64" s="8"/>
       <c r="N64" s="6"/>
@@ -1900,7 +1890,7 @@
       <c r="R64" s="6"/>
       <c r="T64" s="6"/>
     </row>
-    <row r="65" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L65" s="7"/>
       <c r="M65" s="8"/>
       <c r="N65" s="6"/>
@@ -1910,7 +1900,7 @@
       <c r="R65" s="6"/>
       <c r="T65" s="6"/>
     </row>
-    <row r="66" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L66" s="7"/>
       <c r="M66" s="8"/>
       <c r="N66" s="6"/>
@@ -1920,7 +1910,7 @@
       <c r="R66" s="6"/>
       <c r="T66" s="6"/>
     </row>
-    <row r="67" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L67" s="7"/>
       <c r="M67" s="8"/>
       <c r="N67" s="6"/>
@@ -1930,7 +1920,7 @@
       <c r="R67" s="6"/>
       <c r="T67" s="6"/>
     </row>
-    <row r="68" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L68" s="7"/>
       <c r="M68" s="8"/>
       <c r="N68" s="6"/>
@@ -1940,7 +1930,7 @@
       <c r="R68" s="6"/>
       <c r="T68" s="6"/>
     </row>
-    <row r="69" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L69" s="7"/>
       <c r="M69" s="8"/>
       <c r="N69" s="6"/>
@@ -1950,7 +1940,7 @@
       <c r="R69" s="6"/>
       <c r="T69" s="6"/>
     </row>
-    <row r="70" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L70" s="7"/>
       <c r="M70" s="8"/>
       <c r="N70" s="6"/>
@@ -1960,7 +1950,7 @@
       <c r="R70" s="6"/>
       <c r="T70" s="6"/>
     </row>
-    <row r="71" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L71" s="7"/>
       <c r="M71" s="8"/>
       <c r="N71" s="6"/>
@@ -1970,7 +1960,7 @@
       <c r="R71" s="6"/>
       <c r="T71" s="6"/>
     </row>
-    <row r="72" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L72" s="7"/>
       <c r="M72" s="8"/>
       <c r="N72" s="6"/>
@@ -1980,7 +1970,7 @@
       <c r="R72" s="6"/>
       <c r="T72" s="6"/>
     </row>
-    <row r="73" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L73" s="7"/>
       <c r="M73" s="8"/>
       <c r="N73" s="6"/>
@@ -1990,7 +1980,7 @@
       <c r="R73" s="6"/>
       <c r="T73" s="6"/>
     </row>
-    <row r="74" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L74" s="7"/>
       <c r="M74" s="8"/>
       <c r="N74" s="6"/>
@@ -2000,7 +1990,8 @@
       <c r="R74" s="6"/>
       <c r="T74" s="6"/>
     </row>
-    <row r="75" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:20" x14ac:dyDescent="0.45">
+      <c r="C75" s="6"/>
       <c r="L75" s="7"/>
       <c r="M75" s="8"/>
       <c r="N75" s="6"/>
@@ -2010,8 +2001,7 @@
       <c r="R75" s="6"/>
       <c r="T75" s="6"/>
     </row>
-    <row r="76" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C76" s="6"/>
+    <row r="76" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L76" s="7"/>
       <c r="M76" s="8"/>
       <c r="N76" s="6"/>
@@ -2021,7 +2011,7 @@
       <c r="R76" s="6"/>
       <c r="T76" s="6"/>
     </row>
-    <row r="77" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L77" s="7"/>
       <c r="M77" s="8"/>
       <c r="N77" s="6"/>
@@ -2031,7 +2021,7 @@
       <c r="R77" s="6"/>
       <c r="T77" s="6"/>
     </row>
-    <row r="78" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L78" s="7"/>
       <c r="M78" s="8"/>
       <c r="N78" s="6"/>
@@ -2041,7 +2031,7 @@
       <c r="R78" s="6"/>
       <c r="T78" s="6"/>
     </row>
-    <row r="79" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L79" s="7"/>
       <c r="M79" s="8"/>
       <c r="N79" s="6"/>
@@ -2051,7 +2041,7 @@
       <c r="R79" s="6"/>
       <c r="T79" s="6"/>
     </row>
-    <row r="80" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L80" s="7"/>
       <c r="M80" s="8"/>
       <c r="N80" s="6"/>
@@ -2061,9 +2051,12 @@
       <c r="R80" s="6"/>
       <c r="T80" s="6"/>
     </row>
-    <row r="81" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:20" x14ac:dyDescent="0.45">
+      <c r="C81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
       <c r="L81" s="7"/>
-      <c r="M81" s="8"/>
       <c r="N81" s="6"/>
       <c r="O81" s="6"/>
       <c r="P81" s="6"/>
@@ -2071,12 +2064,9 @@
       <c r="R81" s="6"/>
       <c r="T81" s="6"/>
     </row>
-    <row r="82" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C82" s="6"/>
-      <c r="I82" s="6"/>
-      <c r="J82" s="6"/>
-      <c r="K82" s="6"/>
+    <row r="82" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L82" s="7"/>
+      <c r="M82" s="8"/>
       <c r="N82" s="6"/>
       <c r="O82" s="6"/>
       <c r="P82" s="6"/>
@@ -2084,7 +2074,7 @@
       <c r="R82" s="6"/>
       <c r="T82" s="6"/>
     </row>
-    <row r="83" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L83" s="7"/>
       <c r="M83" s="8"/>
       <c r="N83" s="6"/>
@@ -2094,7 +2084,7 @@
       <c r="R83" s="6"/>
       <c r="T83" s="6"/>
     </row>
-    <row r="84" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L84" s="7"/>
       <c r="M84" s="8"/>
       <c r="N84" s="6"/>
@@ -2104,7 +2094,7 @@
       <c r="R84" s="6"/>
       <c r="T84" s="6"/>
     </row>
-    <row r="85" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L85" s="7"/>
       <c r="M85" s="8"/>
       <c r="N85" s="6"/>
@@ -2114,7 +2104,7 @@
       <c r="R85" s="6"/>
       <c r="T85" s="6"/>
     </row>
-    <row r="86" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L86" s="7"/>
       <c r="M86" s="8"/>
       <c r="N86" s="6"/>
@@ -2124,7 +2114,7 @@
       <c r="R86" s="6"/>
       <c r="T86" s="6"/>
     </row>
-    <row r="87" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L87" s="7"/>
       <c r="M87" s="8"/>
       <c r="N87" s="6"/>
@@ -2134,7 +2124,7 @@
       <c r="R87" s="6"/>
       <c r="T87" s="6"/>
     </row>
-    <row r="88" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L88" s="7"/>
       <c r="M88" s="8"/>
       <c r="N88" s="6"/>
@@ -2144,7 +2134,7 @@
       <c r="R88" s="6"/>
       <c r="T88" s="6"/>
     </row>
-    <row r="89" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L89" s="7"/>
       <c r="M89" s="8"/>
       <c r="N89" s="6"/>
@@ -2154,9 +2144,7 @@
       <c r="R89" s="6"/>
       <c r="T89" s="6"/>
     </row>
-    <row r="90" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="L90" s="7"/>
-      <c r="M90" s="8"/>
+    <row r="90" spans="3:20" x14ac:dyDescent="0.45">
       <c r="N90" s="6"/>
       <c r="O90" s="6"/>
       <c r="P90" s="6"/>
@@ -2164,7 +2152,9 @@
       <c r="R90" s="6"/>
       <c r="T90" s="6"/>
     </row>
-    <row r="91" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:20" x14ac:dyDescent="0.45">
+      <c r="L91" s="7"/>
+      <c r="M91" s="8"/>
       <c r="N91" s="6"/>
       <c r="O91" s="6"/>
       <c r="P91" s="6"/>
@@ -2172,7 +2162,7 @@
       <c r="R91" s="6"/>
       <c r="T91" s="6"/>
     </row>
-    <row r="92" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L92" s="7"/>
       <c r="M92" s="8"/>
       <c r="N92" s="6"/>
@@ -2182,7 +2172,7 @@
       <c r="R92" s="6"/>
       <c r="T92" s="6"/>
     </row>
-    <row r="93" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L93" s="7"/>
       <c r="M93" s="8"/>
       <c r="N93" s="6"/>
@@ -2192,7 +2182,7 @@
       <c r="R93" s="6"/>
       <c r="T93" s="6"/>
     </row>
-    <row r="94" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L94" s="7"/>
       <c r="M94" s="8"/>
       <c r="N94" s="6"/>
@@ -2202,7 +2192,7 @@
       <c r="R94" s="6"/>
       <c r="T94" s="6"/>
     </row>
-    <row r="95" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L95" s="7"/>
       <c r="M95" s="8"/>
       <c r="N95" s="6"/>
@@ -2212,7 +2202,7 @@
       <c r="R95" s="6"/>
       <c r="T95" s="6"/>
     </row>
-    <row r="96" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L96" s="7"/>
       <c r="M96" s="8"/>
       <c r="N96" s="6"/>
@@ -2222,7 +2212,7 @@
       <c r="R96" s="6"/>
       <c r="T96" s="6"/>
     </row>
-    <row r="97" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L97" s="7"/>
       <c r="M97" s="8"/>
       <c r="N97" s="6"/>
@@ -2232,7 +2222,7 @@
       <c r="R97" s="6"/>
       <c r="T97" s="6"/>
     </row>
-    <row r="98" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L98" s="7"/>
       <c r="M98" s="8"/>
       <c r="N98" s="6"/>
@@ -2242,7 +2232,7 @@
       <c r="R98" s="6"/>
       <c r="T98" s="6"/>
     </row>
-    <row r="99" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L99" s="7"/>
       <c r="M99" s="8"/>
       <c r="N99" s="6"/>
@@ -2252,7 +2242,7 @@
       <c r="R99" s="6"/>
       <c r="T99" s="6"/>
     </row>
-    <row r="100" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L100" s="7"/>
       <c r="M100" s="8"/>
       <c r="N100" s="6"/>
@@ -2262,7 +2252,7 @@
       <c r="R100" s="6"/>
       <c r="T100" s="6"/>
     </row>
-    <row r="101" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L101" s="7"/>
       <c r="M101" s="8"/>
       <c r="N101" s="6"/>
@@ -2272,7 +2262,7 @@
       <c r="R101" s="6"/>
       <c r="T101" s="6"/>
     </row>
-    <row r="102" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L102" s="7"/>
       <c r="M102" s="8"/>
       <c r="N102" s="6"/>
@@ -2282,7 +2272,7 @@
       <c r="R102" s="6"/>
       <c r="T102" s="6"/>
     </row>
-    <row r="103" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L103" s="7"/>
       <c r="M103" s="8"/>
       <c r="N103" s="6"/>
@@ -2292,9 +2282,8 @@
       <c r="R103" s="6"/>
       <c r="T103" s="6"/>
     </row>
-    <row r="104" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="L104" s="7"/>
-      <c r="M104" s="8"/>
+    <row r="104" spans="3:20" x14ac:dyDescent="0.45">
+      <c r="L104" s="6"/>
       <c r="N104" s="6"/>
       <c r="O104" s="6"/>
       <c r="P104" s="6"/>
@@ -2302,8 +2291,9 @@
       <c r="R104" s="6"/>
       <c r="T104" s="6"/>
     </row>
-    <row r="105" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="L105" s="6"/>
+    <row r="105" spans="3:20" x14ac:dyDescent="0.45">
+      <c r="L105" s="7"/>
+      <c r="M105" s="8"/>
       <c r="N105" s="6"/>
       <c r="O105" s="6"/>
       <c r="P105" s="6"/>
@@ -2311,7 +2301,7 @@
       <c r="R105" s="6"/>
       <c r="T105" s="6"/>
     </row>
-    <row r="106" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L106" s="7"/>
       <c r="M106" s="8"/>
       <c r="N106" s="6"/>
@@ -2321,7 +2311,7 @@
       <c r="R106" s="6"/>
       <c r="T106" s="6"/>
     </row>
-    <row r="107" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L107" s="7"/>
       <c r="M107" s="8"/>
       <c r="N107" s="6"/>
@@ -2331,7 +2321,7 @@
       <c r="R107" s="6"/>
       <c r="T107" s="6"/>
     </row>
-    <row r="108" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L108" s="7"/>
       <c r="M108" s="8"/>
       <c r="N108" s="6"/>
@@ -2341,9 +2331,12 @@
       <c r="R108" s="6"/>
       <c r="T108" s="6"/>
     </row>
-    <row r="109" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="L109" s="7"/>
-      <c r="M109" s="8"/>
+    <row r="109" spans="3:20" x14ac:dyDescent="0.45">
+      <c r="C109" s="6"/>
+      <c r="H109" s="6"/>
+      <c r="I109" s="6"/>
+      <c r="K109" s="6"/>
+      <c r="L109" s="6"/>
       <c r="N109" s="6"/>
       <c r="O109" s="6"/>
       <c r="P109" s="6"/>
@@ -2351,12 +2344,9 @@
       <c r="R109" s="6"/>
       <c r="T109" s="6"/>
     </row>
-    <row r="110" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C110" s="6"/>
-      <c r="H110" s="6"/>
-      <c r="I110" s="6"/>
-      <c r="K110" s="6"/>
-      <c r="L110" s="6"/>
+    <row r="110" spans="3:20" x14ac:dyDescent="0.45">
+      <c r="L110" s="7"/>
+      <c r="M110" s="8"/>
       <c r="N110" s="6"/>
       <c r="O110" s="6"/>
       <c r="P110" s="6"/>
@@ -2364,7 +2354,7 @@
       <c r="R110" s="6"/>
       <c r="T110" s="6"/>
     </row>
-    <row r="111" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L111" s="7"/>
       <c r="M111" s="8"/>
       <c r="N111" s="6"/>
@@ -2374,7 +2364,7 @@
       <c r="R111" s="6"/>
       <c r="T111" s="6"/>
     </row>
-    <row r="112" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L112" s="7"/>
       <c r="M112" s="8"/>
       <c r="N112" s="6"/>
@@ -2384,7 +2374,7 @@
       <c r="R112" s="6"/>
       <c r="T112" s="6"/>
     </row>
-    <row r="113" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="113" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L113" s="7"/>
       <c r="M113" s="8"/>
       <c r="N113" s="6"/>
@@ -2394,7 +2384,7 @@
       <c r="R113" s="6"/>
       <c r="T113" s="6"/>
     </row>
-    <row r="114" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="114" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L114" s="7"/>
       <c r="M114" s="8"/>
       <c r="N114" s="6"/>
@@ -2404,7 +2394,7 @@
       <c r="R114" s="6"/>
       <c r="T114" s="6"/>
     </row>
-    <row r="115" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="115" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L115" s="7"/>
       <c r="M115" s="8"/>
       <c r="N115" s="6"/>
@@ -2414,9 +2404,8 @@
       <c r="R115" s="6"/>
       <c r="T115" s="6"/>
     </row>
-    <row r="116" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="116" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L116" s="7"/>
-      <c r="M116" s="8"/>
       <c r="N116" s="6"/>
       <c r="O116" s="6"/>
       <c r="P116" s="6"/>
@@ -2424,8 +2413,9 @@
       <c r="R116" s="6"/>
       <c r="T116" s="6"/>
     </row>
-    <row r="117" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="117" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L117" s="7"/>
+      <c r="M117" s="8"/>
       <c r="N117" s="6"/>
       <c r="O117" s="6"/>
       <c r="P117" s="6"/>
@@ -2433,7 +2423,7 @@
       <c r="R117" s="6"/>
       <c r="T117" s="6"/>
     </row>
-    <row r="118" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="118" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L118" s="7"/>
       <c r="M118" s="8"/>
       <c r="N118" s="6"/>
@@ -2443,9 +2433,8 @@
       <c r="R118" s="6"/>
       <c r="T118" s="6"/>
     </row>
-    <row r="119" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="119" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L119" s="7"/>
-      <c r="M119" s="8"/>
       <c r="N119" s="6"/>
       <c r="O119" s="6"/>
       <c r="P119" s="6"/>
@@ -2453,7 +2442,7 @@
       <c r="R119" s="6"/>
       <c r="T119" s="6"/>
     </row>
-    <row r="120" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="120" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L120" s="7"/>
       <c r="N120" s="6"/>
       <c r="O120" s="6"/>
@@ -2462,8 +2451,9 @@
       <c r="R120" s="6"/>
       <c r="T120" s="6"/>
     </row>
-    <row r="121" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="121" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L121" s="7"/>
+      <c r="M121" s="8"/>
       <c r="N121" s="6"/>
       <c r="O121" s="6"/>
       <c r="P121" s="6"/>
@@ -2471,9 +2461,8 @@
       <c r="R121" s="6"/>
       <c r="T121" s="6"/>
     </row>
-    <row r="122" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="122" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L122" s="7"/>
-      <c r="M122" s="8"/>
       <c r="N122" s="6"/>
       <c r="O122" s="6"/>
       <c r="P122" s="6"/>
@@ -2481,8 +2470,9 @@
       <c r="R122" s="6"/>
       <c r="T122" s="6"/>
     </row>
-    <row r="123" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="123" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L123" s="7"/>
+      <c r="M123" s="8"/>
       <c r="N123" s="6"/>
       <c r="O123" s="6"/>
       <c r="P123" s="6"/>
@@ -2490,7 +2480,7 @@
       <c r="R123" s="6"/>
       <c r="T123" s="6"/>
     </row>
-    <row r="124" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="124" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L124" s="7"/>
       <c r="M124" s="8"/>
       <c r="N124" s="6"/>
@@ -2500,7 +2490,7 @@
       <c r="R124" s="6"/>
       <c r="T124" s="6"/>
     </row>
-    <row r="125" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="125" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L125" s="7"/>
       <c r="M125" s="8"/>
       <c r="N125" s="6"/>
@@ -2510,28 +2500,27 @@
       <c r="R125" s="6"/>
       <c r="T125" s="6"/>
     </row>
-    <row r="126" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="L126" s="7"/>
-      <c r="M126" s="8"/>
-      <c r="N126" s="6"/>
-      <c r="O126" s="6"/>
-      <c r="P126" s="6"/>
-      <c r="Q126" s="6"/>
-      <c r="R126" s="6"/>
+    <row r="126" spans="8:20" x14ac:dyDescent="0.45">
+      <c r="H126" s="6"/>
+      <c r="I126" s="6"/>
+      <c r="J126" s="6"/>
+      <c r="K126" s="6"/>
+      <c r="L126" s="6"/>
+      <c r="R126" s="7"/>
       <c r="T126" s="6"/>
     </row>
-    <row r="127" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H127" s="6"/>
-      <c r="I127" s="6"/>
-      <c r="J127" s="6"/>
-      <c r="K127" s="6"/>
-      <c r="L127" s="6"/>
-      <c r="R127" s="7"/>
+    <row r="127" spans="8:20" x14ac:dyDescent="0.45">
+      <c r="L127" s="7"/>
+      <c r="M127" s="8"/>
+      <c r="N127" s="6"/>
+      <c r="O127" s="6"/>
+      <c r="P127" s="6"/>
+      <c r="Q127" s="6"/>
+      <c r="R127" s="6"/>
       <c r="T127" s="6"/>
     </row>
-    <row r="128" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="128" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L128" s="7"/>
-      <c r="M128" s="8"/>
       <c r="N128" s="6"/>
       <c r="O128" s="6"/>
       <c r="P128" s="6"/>
@@ -2539,8 +2528,9 @@
       <c r="R128" s="6"/>
       <c r="T128" s="6"/>
     </row>
-    <row r="129" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="129" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L129" s="7"/>
+      <c r="M129" s="8"/>
       <c r="N129" s="6"/>
       <c r="O129" s="6"/>
       <c r="P129" s="6"/>
@@ -2548,9 +2538,8 @@
       <c r="R129" s="6"/>
       <c r="T129" s="6"/>
     </row>
-    <row r="130" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="L130" s="7"/>
-      <c r="M130" s="8"/>
+    <row r="130" spans="8:20" x14ac:dyDescent="0.45">
+      <c r="H130" s="6"/>
       <c r="N130" s="6"/>
       <c r="O130" s="6"/>
       <c r="P130" s="6"/>
@@ -2558,8 +2547,9 @@
       <c r="R130" s="6"/>
       <c r="T130" s="6"/>
     </row>
-    <row r="131" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H131" s="6"/>
+    <row r="131" spans="8:20" x14ac:dyDescent="0.45">
+      <c r="L131" s="7"/>
+      <c r="M131" s="8"/>
       <c r="N131" s="6"/>
       <c r="O131" s="6"/>
       <c r="P131" s="6"/>
@@ -2567,7 +2557,7 @@
       <c r="R131" s="6"/>
       <c r="T131" s="6"/>
     </row>
-    <row r="132" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="132" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L132" s="7"/>
       <c r="M132" s="8"/>
       <c r="N132" s="6"/>
@@ -2577,7 +2567,7 @@
       <c r="R132" s="6"/>
       <c r="T132" s="6"/>
     </row>
-    <row r="133" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="133" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L133" s="7"/>
       <c r="M133" s="8"/>
       <c r="N133" s="6"/>
@@ -2587,7 +2577,7 @@
       <c r="R133" s="6"/>
       <c r="T133" s="6"/>
     </row>
-    <row r="134" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="134" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L134" s="7"/>
       <c r="M134" s="8"/>
       <c r="N134" s="6"/>
@@ -2597,7 +2587,7 @@
       <c r="R134" s="6"/>
       <c r="T134" s="6"/>
     </row>
-    <row r="135" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="135" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L135" s="7"/>
       <c r="M135" s="8"/>
       <c r="N135" s="6"/>
@@ -2607,7 +2597,7 @@
       <c r="R135" s="6"/>
       <c r="T135" s="6"/>
     </row>
-    <row r="136" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="136" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L136" s="7"/>
       <c r="M136" s="8"/>
       <c r="N136" s="6"/>
@@ -2617,7 +2607,7 @@
       <c r="R136" s="6"/>
       <c r="T136" s="6"/>
     </row>
-    <row r="137" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="137" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L137" s="7"/>
       <c r="M137" s="8"/>
       <c r="N137" s="6"/>
@@ -2627,7 +2617,7 @@
       <c r="R137" s="6"/>
       <c r="T137" s="6"/>
     </row>
-    <row r="138" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="138" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L138" s="7"/>
       <c r="M138" s="8"/>
       <c r="N138" s="6"/>
@@ -2637,7 +2627,7 @@
       <c r="R138" s="6"/>
       <c r="T138" s="6"/>
     </row>
-    <row r="139" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="139" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L139" s="7"/>
       <c r="M139" s="8"/>
       <c r="N139" s="6"/>
@@ -2647,7 +2637,7 @@
       <c r="R139" s="6"/>
       <c r="T139" s="6"/>
     </row>
-    <row r="140" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="140" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L140" s="7"/>
       <c r="M140" s="8"/>
       <c r="N140" s="6"/>
@@ -2657,7 +2647,7 @@
       <c r="R140" s="6"/>
       <c r="T140" s="6"/>
     </row>
-    <row r="141" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="141" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L141" s="7"/>
       <c r="M141" s="8"/>
       <c r="N141" s="6"/>
@@ -2667,7 +2657,7 @@
       <c r="R141" s="6"/>
       <c r="T141" s="6"/>
     </row>
-    <row r="142" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="142" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L142" s="7"/>
       <c r="M142" s="8"/>
       <c r="N142" s="6"/>
@@ -2677,7 +2667,7 @@
       <c r="R142" s="6"/>
       <c r="T142" s="6"/>
     </row>
-    <row r="143" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="143" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L143" s="7"/>
       <c r="M143" s="8"/>
       <c r="N143" s="6"/>
@@ -2687,7 +2677,7 @@
       <c r="R143" s="6"/>
       <c r="T143" s="6"/>
     </row>
-    <row r="144" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="144" spans="8:20" x14ac:dyDescent="0.45">
       <c r="L144" s="7"/>
       <c r="M144" s="8"/>
       <c r="N144" s="6"/>
@@ -2697,7 +2687,7 @@
       <c r="R144" s="6"/>
       <c r="T144" s="6"/>
     </row>
-    <row r="145" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L145" s="7"/>
       <c r="M145" s="8"/>
       <c r="N145" s="6"/>
@@ -2707,7 +2697,7 @@
       <c r="R145" s="6"/>
       <c r="T145" s="6"/>
     </row>
-    <row r="146" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L146" s="7"/>
       <c r="M146" s="8"/>
       <c r="N146" s="6"/>
@@ -2717,9 +2707,13 @@
       <c r="R146" s="6"/>
       <c r="T146" s="6"/>
     </row>
-    <row r="147" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="L147" s="7"/>
-      <c r="M147" s="8"/>
+    <row r="147" spans="3:20" x14ac:dyDescent="0.45">
+      <c r="C147" s="6"/>
+      <c r="H147" s="6"/>
+      <c r="I147" s="6"/>
+      <c r="J147" s="6"/>
+      <c r="K147" s="6"/>
+      <c r="L147" s="6"/>
       <c r="N147" s="6"/>
       <c r="O147" s="6"/>
       <c r="P147" s="6"/>
@@ -2727,7 +2721,7 @@
       <c r="R147" s="6"/>
       <c r="T147" s="6"/>
     </row>
-    <row r="148" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:20" x14ac:dyDescent="0.45">
       <c r="C148" s="6"/>
       <c r="H148" s="6"/>
       <c r="I148" s="6"/>
@@ -2741,13 +2735,9 @@
       <c r="R148" s="6"/>
       <c r="T148" s="6"/>
     </row>
-    <row r="149" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C149" s="6"/>
-      <c r="H149" s="6"/>
-      <c r="I149" s="6"/>
-      <c r="J149" s="6"/>
-      <c r="K149" s="6"/>
-      <c r="L149" s="6"/>
+    <row r="149" spans="3:20" x14ac:dyDescent="0.45">
+      <c r="L149" s="7"/>
+      <c r="M149" s="8"/>
       <c r="N149" s="6"/>
       <c r="O149" s="6"/>
       <c r="P149" s="6"/>
@@ -2755,7 +2745,7 @@
       <c r="R149" s="6"/>
       <c r="T149" s="6"/>
     </row>
-    <row r="150" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="150" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L150" s="7"/>
       <c r="M150" s="8"/>
       <c r="N150" s="6"/>
@@ -2765,7 +2755,7 @@
       <c r="R150" s="6"/>
       <c r="T150" s="6"/>
     </row>
-    <row r="151" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="151" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L151" s="7"/>
       <c r="M151" s="8"/>
       <c r="N151" s="6"/>
@@ -2775,7 +2765,7 @@
       <c r="R151" s="6"/>
       <c r="T151" s="6"/>
     </row>
-    <row r="152" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="152" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L152" s="7"/>
       <c r="M152" s="8"/>
       <c r="N152" s="6"/>
@@ -2785,7 +2775,7 @@
       <c r="R152" s="6"/>
       <c r="T152" s="6"/>
     </row>
-    <row r="153" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="153" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L153" s="7"/>
       <c r="M153" s="8"/>
       <c r="N153" s="6"/>
@@ -2795,7 +2785,7 @@
       <c r="R153" s="6"/>
       <c r="T153" s="6"/>
     </row>
-    <row r="154" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="154" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L154" s="7"/>
       <c r="M154" s="8"/>
       <c r="N154" s="6"/>
@@ -2805,9 +2795,12 @@
       <c r="R154" s="6"/>
       <c r="T154" s="6"/>
     </row>
-    <row r="155" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="155" spans="3:20" x14ac:dyDescent="0.45">
+      <c r="C155" s="6"/>
+      <c r="I155" s="6"/>
+      <c r="J155" s="6"/>
+      <c r="K155" s="6"/>
       <c r="L155" s="7"/>
-      <c r="M155" s="8"/>
       <c r="N155" s="6"/>
       <c r="O155" s="6"/>
       <c r="P155" s="6"/>
@@ -2815,12 +2808,9 @@
       <c r="R155" s="6"/>
       <c r="T155" s="6"/>
     </row>
-    <row r="156" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C156" s="6"/>
-      <c r="I156" s="6"/>
-      <c r="J156" s="6"/>
-      <c r="K156" s="6"/>
+    <row r="156" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L156" s="7"/>
+      <c r="M156" s="8"/>
       <c r="N156" s="6"/>
       <c r="O156" s="6"/>
       <c r="P156" s="6"/>
@@ -2828,7 +2818,7 @@
       <c r="R156" s="6"/>
       <c r="T156" s="6"/>
     </row>
-    <row r="157" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="157" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L157" s="7"/>
       <c r="M157" s="8"/>
       <c r="N157" s="6"/>
@@ -2838,7 +2828,7 @@
       <c r="R157" s="6"/>
       <c r="T157" s="6"/>
     </row>
-    <row r="158" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="158" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L158" s="7"/>
       <c r="M158" s="8"/>
       <c r="N158" s="6"/>
@@ -2848,7 +2838,7 @@
       <c r="R158" s="6"/>
       <c r="T158" s="6"/>
     </row>
-    <row r="159" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="159" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L159" s="7"/>
       <c r="M159" s="8"/>
       <c r="N159" s="6"/>
@@ -2858,7 +2848,7 @@
       <c r="R159" s="6"/>
       <c r="T159" s="6"/>
     </row>
-    <row r="160" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="160" spans="3:20" x14ac:dyDescent="0.45">
       <c r="L160" s="7"/>
       <c r="M160" s="8"/>
       <c r="N160" s="6"/>
@@ -2868,7 +2858,7 @@
       <c r="R160" s="6"/>
       <c r="T160" s="6"/>
     </row>
-    <row r="161" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="161" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L161" s="7"/>
       <c r="M161" s="8"/>
       <c r="N161" s="6"/>
@@ -2878,7 +2868,7 @@
       <c r="R161" s="6"/>
       <c r="T161" s="6"/>
     </row>
-    <row r="162" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="162" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L162" s="7"/>
       <c r="M162" s="8"/>
       <c r="N162" s="6"/>
@@ -2888,7 +2878,7 @@
       <c r="R162" s="6"/>
       <c r="T162" s="6"/>
     </row>
-    <row r="163" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="163" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L163" s="7"/>
       <c r="M163" s="8"/>
       <c r="N163" s="6"/>
@@ -2898,7 +2888,7 @@
       <c r="R163" s="6"/>
       <c r="T163" s="6"/>
     </row>
-    <row r="164" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="164" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L164" s="7"/>
       <c r="M164" s="8"/>
       <c r="N164" s="6"/>
@@ -2908,7 +2898,7 @@
       <c r="R164" s="6"/>
       <c r="T164" s="6"/>
     </row>
-    <row r="165" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="165" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L165" s="7"/>
       <c r="M165" s="8"/>
       <c r="N165" s="6"/>
@@ -2918,7 +2908,7 @@
       <c r="R165" s="6"/>
       <c r="T165" s="6"/>
     </row>
-    <row r="166" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="166" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L166" s="7"/>
       <c r="M166" s="8"/>
       <c r="N166" s="6"/>
@@ -2928,9 +2918,7 @@
       <c r="R166" s="6"/>
       <c r="T166" s="6"/>
     </row>
-    <row r="167" spans="12:20" x14ac:dyDescent="0.25">
-      <c r="L167" s="7"/>
-      <c r="M167" s="8"/>
+    <row r="167" spans="12:20" x14ac:dyDescent="0.45">
       <c r="N167" s="6"/>
       <c r="O167" s="6"/>
       <c r="P167" s="6"/>
@@ -2938,7 +2926,9 @@
       <c r="R167" s="6"/>
       <c r="T167" s="6"/>
     </row>
-    <row r="168" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="168" spans="12:20" x14ac:dyDescent="0.45">
+      <c r="L168" s="7"/>
+      <c r="M168" s="8"/>
       <c r="N168" s="6"/>
       <c r="O168" s="6"/>
       <c r="P168" s="6"/>
@@ -2946,7 +2936,7 @@
       <c r="R168" s="6"/>
       <c r="T168" s="6"/>
     </row>
-    <row r="169" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="169" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L169" s="7"/>
       <c r="M169" s="8"/>
       <c r="N169" s="6"/>
@@ -2956,7 +2946,7 @@
       <c r="R169" s="6"/>
       <c r="T169" s="6"/>
     </row>
-    <row r="170" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="170" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L170" s="7"/>
       <c r="M170" s="8"/>
       <c r="N170" s="6"/>
@@ -2966,7 +2956,7 @@
       <c r="R170" s="6"/>
       <c r="T170" s="6"/>
     </row>
-    <row r="171" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="171" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L171" s="7"/>
       <c r="M171" s="8"/>
       <c r="N171" s="6"/>
@@ -2976,7 +2966,7 @@
       <c r="R171" s="6"/>
       <c r="T171" s="6"/>
     </row>
-    <row r="172" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="172" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L172" s="7"/>
       <c r="M172" s="8"/>
       <c r="N172" s="6"/>
@@ -2986,7 +2976,7 @@
       <c r="R172" s="6"/>
       <c r="T172" s="6"/>
     </row>
-    <row r="173" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="173" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L173" s="7"/>
       <c r="M173" s="8"/>
       <c r="N173" s="6"/>
@@ -2996,7 +2986,7 @@
       <c r="R173" s="6"/>
       <c r="T173" s="6"/>
     </row>
-    <row r="174" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="174" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L174" s="7"/>
       <c r="M174" s="8"/>
       <c r="N174" s="6"/>
@@ -3006,9 +2996,7 @@
       <c r="R174" s="6"/>
       <c r="T174" s="6"/>
     </row>
-    <row r="175" spans="12:20" x14ac:dyDescent="0.25">
-      <c r="L175" s="7"/>
-      <c r="M175" s="8"/>
+    <row r="175" spans="12:20" x14ac:dyDescent="0.45">
       <c r="N175" s="6"/>
       <c r="O175" s="6"/>
       <c r="P175" s="6"/>
@@ -3016,7 +3004,9 @@
       <c r="R175" s="6"/>
       <c r="T175" s="6"/>
     </row>
-    <row r="176" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="176" spans="12:20" x14ac:dyDescent="0.45">
+      <c r="L176" s="7"/>
+      <c r="M176" s="8"/>
       <c r="N176" s="6"/>
       <c r="O176" s="6"/>
       <c r="P176" s="6"/>
@@ -3024,7 +3014,7 @@
       <c r="R176" s="6"/>
       <c r="T176" s="6"/>
     </row>
-    <row r="177" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="177" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L177" s="7"/>
       <c r="M177" s="8"/>
       <c r="N177" s="6"/>
@@ -3034,9 +3024,8 @@
       <c r="R177" s="6"/>
       <c r="T177" s="6"/>
     </row>
-    <row r="178" spans="12:20" x14ac:dyDescent="0.25">
-      <c r="L178" s="7"/>
-      <c r="M178" s="8"/>
+    <row r="178" spans="12:20" x14ac:dyDescent="0.45">
+      <c r="L178" s="6"/>
       <c r="N178" s="6"/>
       <c r="O178" s="6"/>
       <c r="P178" s="6"/>
@@ -3044,8 +3033,9 @@
       <c r="R178" s="6"/>
       <c r="T178" s="6"/>
     </row>
-    <row r="179" spans="12:20" x14ac:dyDescent="0.25">
-      <c r="L179" s="6"/>
+    <row r="179" spans="12:20" x14ac:dyDescent="0.45">
+      <c r="L179" s="7"/>
+      <c r="M179" s="8"/>
       <c r="N179" s="6"/>
       <c r="O179" s="6"/>
       <c r="P179" s="6"/>
@@ -3053,7 +3043,7 @@
       <c r="R179" s="6"/>
       <c r="T179" s="6"/>
     </row>
-    <row r="180" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="180" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L180" s="7"/>
       <c r="M180" s="8"/>
       <c r="N180" s="6"/>
@@ -3063,24 +3053,24 @@
       <c r="R180" s="6"/>
       <c r="T180" s="6"/>
     </row>
-    <row r="181" spans="12:20" x14ac:dyDescent="0.25">
-      <c r="L181" s="7"/>
-      <c r="M181" s="8"/>
+    <row r="181" spans="12:20" x14ac:dyDescent="0.45">
       <c r="N181" s="6"/>
       <c r="O181" s="6"/>
       <c r="P181" s="6"/>
       <c r="Q181" s="6"/>
-      <c r="R181" s="6"/>
       <c r="T181" s="6"/>
     </row>
-    <row r="182" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="182" spans="12:20" x14ac:dyDescent="0.45">
+      <c r="L182" s="7"/>
+      <c r="M182" s="8"/>
       <c r="N182" s="6"/>
       <c r="O182" s="6"/>
       <c r="P182" s="6"/>
       <c r="Q182" s="6"/>
+      <c r="R182" s="6"/>
       <c r="T182" s="6"/>
     </row>
-    <row r="183" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="183" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L183" s="7"/>
       <c r="M183" s="8"/>
       <c r="N183" s="6"/>
@@ -3090,24 +3080,24 @@
       <c r="R183" s="6"/>
       <c r="T183" s="6"/>
     </row>
-    <row r="184" spans="12:20" x14ac:dyDescent="0.25">
-      <c r="L184" s="7"/>
-      <c r="M184" s="8"/>
+    <row r="184" spans="12:20" x14ac:dyDescent="0.45">
       <c r="N184" s="6"/>
       <c r="O184" s="6"/>
       <c r="P184" s="6"/>
       <c r="Q184" s="6"/>
-      <c r="R184" s="6"/>
       <c r="T184" s="6"/>
     </row>
-    <row r="185" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="185" spans="12:20" x14ac:dyDescent="0.45">
       <c r="N185" s="6"/>
       <c r="O185" s="6"/>
       <c r="P185" s="6"/>
       <c r="Q185" s="6"/>
+      <c r="R185" s="6"/>
       <c r="T185" s="6"/>
     </row>
-    <row r="186" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="186" spans="12:20" x14ac:dyDescent="0.45">
+      <c r="L186" s="7"/>
+      <c r="M186" s="8"/>
       <c r="N186" s="6"/>
       <c r="O186" s="6"/>
       <c r="P186" s="6"/>
@@ -3115,7 +3105,7 @@
       <c r="R186" s="6"/>
       <c r="T186" s="6"/>
     </row>
-    <row r="187" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="187" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L187" s="7"/>
       <c r="M187" s="8"/>
       <c r="N187" s="6"/>
@@ -3125,7 +3115,7 @@
       <c r="R187" s="6"/>
       <c r="T187" s="6"/>
     </row>
-    <row r="188" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="188" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L188" s="7"/>
       <c r="M188" s="8"/>
       <c r="N188" s="6"/>
@@ -3135,8 +3125,7 @@
       <c r="R188" s="6"/>
       <c r="T188" s="6"/>
     </row>
-    <row r="189" spans="12:20" x14ac:dyDescent="0.25">
-      <c r="L189" s="7"/>
+    <row r="189" spans="12:20" x14ac:dyDescent="0.45">
       <c r="M189" s="8"/>
       <c r="N189" s="6"/>
       <c r="O189" s="6"/>
@@ -3145,7 +3134,8 @@
       <c r="R189" s="6"/>
       <c r="T189" s="6"/>
     </row>
-    <row r="190" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="190" spans="12:20" x14ac:dyDescent="0.45">
+      <c r="L190" s="7"/>
       <c r="M190" s="8"/>
       <c r="N190" s="6"/>
       <c r="O190" s="6"/>
@@ -3154,7 +3144,7 @@
       <c r="R190" s="6"/>
       <c r="T190" s="6"/>
     </row>
-    <row r="191" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="191" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L191" s="7"/>
       <c r="M191" s="8"/>
       <c r="N191" s="6"/>
@@ -3164,7 +3154,7 @@
       <c r="R191" s="6"/>
       <c r="T191" s="6"/>
     </row>
-    <row r="192" spans="12:20" x14ac:dyDescent="0.25">
+    <row r="192" spans="12:20" x14ac:dyDescent="0.45">
       <c r="L192" s="7"/>
       <c r="M192" s="8"/>
       <c r="N192" s="6"/>
@@ -3174,16 +3164,6 @@
       <c r="R192" s="6"/>
       <c r="T192" s="6"/>
     </row>
-    <row r="193" spans="12:20" x14ac:dyDescent="0.25">
-      <c r="L193" s="7"/>
-      <c r="M193" s="8"/>
-      <c r="N193" s="6"/>
-      <c r="O193" s="6"/>
-      <c r="P193" s="6"/>
-      <c r="Q193" s="6"/>
-      <c r="R193" s="6"/>
-      <c r="T193" s="6"/>
-    </row>
   </sheetData>
   <sortState ref="A3:T8">
     <sortCondition ref="C3:C8"/>

</xml_diff>